<commit_message>
Updated user stories to be more precise.
</commit_message>
<xml_diff>
--- a/User_Stories.xlsx
+++ b/User_Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo De Dios\Desktop\COMP0035\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BB091C-62B7-4613-B35B-6815336D89AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675CDA8E-EB04-44BF-B0B6-68DE328D5C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile User Story Template'!$B$1:$E$21</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>CLICK HERE TO CREATE IN SMARTSHEET</t>
   </si>
@@ -105,46 +114,85 @@
     <t>Film Producer</t>
   </si>
   <si>
-    <t xml:space="preserve">Browse other producer's projects </t>
-  </si>
-  <si>
-    <t>Safely share my project proposal</t>
-  </si>
-  <si>
-    <t>Properly and easily understand it.</t>
-  </si>
-  <si>
-    <t>Be reached by other producers interested in my project.</t>
-  </si>
-  <si>
-    <t>Contact the producers if I am interested in collaborating.</t>
-  </si>
-  <si>
-    <t>Have the data laid out in a clear manner</t>
-  </si>
-  <si>
-    <t>Find different types of graphs</t>
-  </si>
-  <si>
-    <t>Obtain a deeper understanding of film tendencies.</t>
-  </si>
-  <si>
     <t>Advertiser</t>
   </si>
   <si>
-    <t>Ensure that my add slot is visible enough</t>
-  </si>
-  <si>
     <t>Maximize the number of users that see our promotion.</t>
   </si>
   <si>
-    <t>Investor</t>
-  </si>
-  <si>
-    <t>Buy company stocks</t>
-  </si>
-  <si>
     <t>Gain money if the company experiences financial growth.</t>
+  </si>
+  <si>
+    <t>Easily find the types of project my company is interested in.</t>
+  </si>
+  <si>
+    <t>Filter the project proposals by different categories (expected budget, length, genres, etc.)</t>
+  </si>
+  <si>
+    <t>Obtain the detailed information about the producer (years of experience, production company, studies, etc.)</t>
+  </si>
+  <si>
+    <t>Reach out the them if I am interested in a potential collaboration.</t>
+  </si>
+  <si>
+    <t>Be contacted by other producers interested in it.</t>
+  </si>
+  <si>
+    <t>Share my proposal while maintaining my rights to it</t>
+  </si>
+  <si>
+    <t>Customize the graphs (e.g. focus on a specific period, remove certain genres or movies from distributors that I am not interested in, have the revenue in a logarithmic scale, increase the font size of the labels, etc.)</t>
+  </si>
+  <si>
+    <t>Have my graphs laid out in a way that facilitates the research that I want to conduct.</t>
+  </si>
+  <si>
+    <t>View different types of graphs (pie charts, bar and linear plots) that display the correlation between different variables (i.e. revenue, genre, ratings, distribution companies, runtime)</t>
+  </si>
+  <si>
+    <t>Have enough information to carry out my desired research.</t>
+  </si>
+  <si>
+    <t>Include them in the research paper that I will be producing, or show it to my boss to enage in discussion.</t>
+  </si>
+  <si>
+    <t>Ask any questions I may have regarding the use, performance or data protection of the App.</t>
+  </si>
+  <si>
+    <t>Be able to contact the customer support team (either via email or a phone call)</t>
+  </si>
+  <si>
+    <t>Save/Download graphs in various formats (png, jpg, jpeg, tif, etc.)</t>
+  </si>
+  <si>
+    <t>Stop being contacted about it when my company has already decided which other production will be collaborating with us.</t>
+  </si>
+  <si>
+    <t>Remove any of my proposals from the forum</t>
+  </si>
+  <si>
+    <t>Have the option to either freeze or delete my account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop using the app for a period of time or indefinitely. </t>
+  </si>
+  <si>
+    <t>Passive Investor</t>
+  </si>
+  <si>
+    <t>Active Investor</t>
+  </si>
+  <si>
+    <t>Negotiate a position in the director's board, have the right to vote on important business decisions and be informed about them, etc.</t>
+  </si>
+  <si>
+    <t>Buy a small amount of company stock</t>
+  </si>
+  <si>
+    <t>But a significant amount of company stock</t>
+  </si>
+  <si>
+    <t>Ensure that my add slot is visible and displayed regularly (in case there are multiple ads being shown by the app)</t>
   </si>
 </sst>
 </file>
@@ -808,8 +856,8 @@
   <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -858,10 +906,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -874,16 +922,17 @@
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="12">
+        <f>B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -896,16 +945,17 @@
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="12">
+        <f>B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -916,18 +966,19 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="12">
+        <f t="shared" ref="B6:B14" si="0">B5+1</f>
         <v>4</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -938,12 +989,13 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>17</v>
@@ -960,18 +1012,19 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -983,10 +1036,19 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="B9" s="12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -997,10 +1059,19 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
+      <c r="B10" s="12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1011,10 +1082,19 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1025,10 +1105,19 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="B12" s="12">
+        <f>B11+1</f>
+        <v>10</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1039,10 +1128,19 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
+      <c r="B13" s="12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1052,11 +1150,20 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
+    <row r="14" spans="1:13" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>

</xml_diff>